<commit_message>
Update OnSSET input files
</commit_message>
<xml_diff>
--- a/model/OnSSET_Input/amb/burkina-specs-amb.xlsx
+++ b/model/OnSSET_Input/amb/burkina-specs-amb.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5232" yWindow="3816" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="1" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-96" yWindow="600" windowWidth="11712" windowHeight="12456" tabRatio="500" firstSheet="1" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +11,7 @@
     <sheet name="SpecsData" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -21,20 +21,21 @@
   <fonts count="4">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Cambria"/>
+      <charset val="1"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -97,7 +98,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -174,10 +175,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -215,116 +216,52 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -332,33 +269,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -371,13 +299,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -387,15 +309,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -403,7 +323,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -411,22 +330,17 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -436,65 +350,65 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI6"/>
+  <dimension ref="A1:BM6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="AH1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:BM6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="8" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="17" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="32.109375" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="27.21875" bestFit="1" customWidth="1" min="4" max="5"/>
-    <col width="28" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="13.5546875" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="10.88671875" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="22.109375" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="20.44140625" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="12.44140625" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="15.77734375" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="26.44140625" bestFit="1" customWidth="1" min="13" max="13"/>
-    <col width="18.33203125" bestFit="1" customWidth="1" min="14" max="14"/>
-    <col width="16.33203125" bestFit="1" customWidth="1" min="15" max="16"/>
-    <col width="20.33203125" bestFit="1" customWidth="1" min="17" max="17"/>
-    <col width="25.21875" bestFit="1" customWidth="1" min="18" max="18"/>
-    <col width="31" bestFit="1" customWidth="1" min="19" max="19"/>
-    <col width="31.21875" bestFit="1" customWidth="1" min="20" max="20"/>
-    <col width="19.88671875" bestFit="1" customWidth="1" min="21" max="21"/>
-    <col width="22.88671875" bestFit="1" customWidth="1" min="22" max="22"/>
-    <col width="18.21875" bestFit="1" customWidth="1" min="23" max="23"/>
-    <col width="20.88671875" bestFit="1" customWidth="1" min="24" max="24"/>
-    <col width="19.6640625" bestFit="1" customWidth="1" min="25" max="25"/>
-    <col width="24.5546875" bestFit="1" customWidth="1" min="26" max="26"/>
-    <col width="30.33203125" bestFit="1" customWidth="1" min="27" max="27"/>
-    <col width="30.5546875" bestFit="1" customWidth="1" min="28" max="28"/>
-    <col width="19.21875" bestFit="1" customWidth="1" min="29" max="29"/>
-    <col width="17.5546875" bestFit="1" customWidth="1" min="30" max="30"/>
-    <col width="20.21875" bestFit="1" customWidth="1" min="31" max="31"/>
-    <col width="17.5546875" bestFit="1" customWidth="1" min="32" max="32"/>
-    <col width="22.44140625" bestFit="1" customWidth="1" min="33" max="33"/>
-    <col width="28.109375" bestFit="1" customWidth="1" min="34" max="34"/>
-    <col width="28.33203125" bestFit="1" customWidth="1" min="35" max="35"/>
-    <col width="17" bestFit="1" customWidth="1" min="36" max="36"/>
-    <col width="15.33203125" bestFit="1" customWidth="1" min="37" max="37"/>
-    <col width="18.109375" bestFit="1" customWidth="1" min="38" max="38"/>
-    <col width="23.6640625" bestFit="1" customWidth="1" min="39" max="39"/>
-    <col width="15.88671875" bestFit="1" customWidth="1" min="40" max="40"/>
-    <col width="12.5546875" bestFit="1" customWidth="1" min="41" max="41"/>
-    <col width="14.5546875" bestFit="1" customWidth="1" min="42" max="42"/>
-    <col width="20.33203125" bestFit="1" customWidth="1" min="43" max="43"/>
-    <col width="25.21875" bestFit="1" customWidth="1" min="44" max="44"/>
-    <col width="31" bestFit="1" customWidth="1" min="45" max="45"/>
-    <col width="31.21875" bestFit="1" customWidth="1" min="46" max="46"/>
-    <col width="19.88671875" bestFit="1" customWidth="1" min="47" max="47"/>
-    <col width="18.21875" bestFit="1" customWidth="1" min="48" max="48"/>
-    <col width="20.88671875" bestFit="1" customWidth="1" min="49" max="49"/>
-    <col width="27.44140625" bestFit="1" customWidth="1" min="51" max="51"/>
-    <col width="17.21875" bestFit="1" customWidth="1" min="52" max="52"/>
-    <col width="14.44140625" bestFit="1" customWidth="1" min="53" max="53"/>
-    <col width="16.109375" bestFit="1" customWidth="1" min="54" max="54"/>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="32.109375" customWidth="1" min="3" max="3"/>
+    <col width="27.21875" customWidth="1" min="4" max="5"/>
+    <col width="28" customWidth="1" min="6" max="6"/>
+    <col width="13.5546875" customWidth="1" min="7" max="7"/>
+    <col width="10.88671875" customWidth="1" min="8" max="8"/>
+    <col width="22.109375" customWidth="1" min="9" max="9"/>
+    <col width="20.44140625" customWidth="1" min="10" max="10"/>
+    <col width="12.44140625" customWidth="1" min="11" max="11"/>
+    <col width="15.77734375" customWidth="1" min="12" max="12"/>
+    <col width="26.44140625" customWidth="1" min="13" max="13"/>
+    <col width="18.33203125" customWidth="1" min="14" max="14"/>
+    <col width="16.33203125" customWidth="1" min="15" max="16"/>
+    <col width="20.33203125" customWidth="1" min="17" max="17"/>
+    <col width="25.21875" customWidth="1" min="18" max="18"/>
+    <col width="31" customWidth="1" min="19" max="19"/>
+    <col width="31.21875" customWidth="1" min="20" max="20"/>
+    <col width="19.88671875" customWidth="1" min="21" max="21"/>
+    <col width="22.88671875" customWidth="1" min="22" max="22"/>
+    <col width="18.21875" customWidth="1" min="23" max="23"/>
+    <col width="20.88671875" customWidth="1" min="24" max="24"/>
+    <col width="19.6640625" customWidth="1" min="25" max="25"/>
+    <col width="24.5546875" customWidth="1" min="26" max="26"/>
+    <col width="30.33203125" customWidth="1" min="27" max="27"/>
+    <col width="30.5546875" customWidth="1" min="28" max="28"/>
+    <col width="19.21875" customWidth="1" min="29" max="29"/>
+    <col width="17.5546875" customWidth="1" min="30" max="30"/>
+    <col width="20.21875" customWidth="1" min="31" max="31"/>
+    <col width="17.5546875" customWidth="1" min="32" max="32"/>
+    <col width="22.44140625" customWidth="1" min="33" max="33"/>
+    <col width="28.109375" customWidth="1" min="34" max="34"/>
+    <col width="28.33203125" customWidth="1" min="35" max="35"/>
+    <col width="17" customWidth="1" min="36" max="36"/>
+    <col width="15.33203125" customWidth="1" min="37" max="37"/>
+    <col width="18.109375" customWidth="1" min="38" max="38"/>
+    <col width="23.6640625" customWidth="1" min="39" max="39"/>
+    <col width="15.88671875" customWidth="1" min="40" max="40"/>
+    <col width="12.5546875" customWidth="1" min="41" max="41"/>
+    <col width="14.5546875" customWidth="1" min="42" max="42"/>
+    <col width="20.33203125" customWidth="1" min="43" max="43"/>
+    <col width="25.21875" customWidth="1" min="44" max="44"/>
+    <col width="31" customWidth="1" min="45" max="45"/>
+    <col width="31.21875" customWidth="1" min="46" max="46"/>
+    <col width="19.88671875" customWidth="1" min="47" max="47"/>
+    <col width="18.21875" customWidth="1" min="48" max="48"/>
+    <col width="20.88671875" customWidth="1" min="49" max="49"/>
+    <col width="27.44140625" customWidth="1" min="51" max="51"/>
+    <col width="17.21875" customWidth="1" min="52" max="52"/>
+    <col width="14.44140625" customWidth="1" min="53" max="53"/>
+    <col width="16.109375" customWidth="1" min="54" max="54"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -705,100 +619,120 @@
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>SAPV_capital_cost</t>
+          <t>SAPV_capital_cost_Inf</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
+          <t>SAPV_capital_cost_1kW</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>SAPV_capital_cost_100W</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>SAPV_capital_cost_50W</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>SAPV_capital_cost_20W</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
           <t>MGDiesel_OM_TDLines</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>MGDiesel_distribution_losses</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>MGDiesel_connection_cost_per_HH</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>MGDiesel_base_to_peak_load_ratio</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>MGDiesel_capital_cost</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>MGDiesel_OM_costs</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>MGDiesel_technical_life</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>MGDiesel_capacity_factor</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>SADiesel_base_to_peak_load_ratio</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>SADiesel_technical_life</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>SADiesel_OM_costs</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>SADiesel_capital_cost</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>SADiesel_capacity_factor</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>SADiesel_efficiency</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>SADiesel_truck_consumption</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>SADiesel_truck_volume</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>MGDiesel_efficiency</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>MGDiesel_truck_consumption</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>MGDiesel_truck_volume</t>
         </is>
@@ -988,6 +922,18 @@
       <c r="BI2" t="n">
         <v>0</v>
       </c>
+      <c r="BJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1173,6 +1119,18 @@
       <c r="BI3" t="n">
         <v>1</v>
       </c>
+      <c r="BJ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1358,6 +1316,18 @@
       <c r="BI4" t="n">
         <v>2</v>
       </c>
+      <c r="BJ4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1543,6 +1513,18 @@
       <c r="BI5" t="n">
         <v>3</v>
       </c>
+      <c r="BJ5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1728,9 +1710,22 @@
       <c r="BI6" t="n">
         <v>4</v>
       </c>
+      <c r="BJ6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -1740,7 +1735,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BL6"/>
+  <dimension ref="A1:BP6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1971,100 +1966,120 @@
       </c>
       <c r="AS1" s="2" t="inlineStr">
         <is>
-          <t>SAPVCapitalCost</t>
+          <t>SAPVCapitalCostInf</t>
         </is>
       </c>
       <c r="AT1" s="2" t="inlineStr">
         <is>
+          <t>SAPVCapitalCost1kW</t>
+        </is>
+      </c>
+      <c r="AU1" s="2" t="inlineStr">
+        <is>
+          <t>SAPVCapitalCost100W</t>
+        </is>
+      </c>
+      <c r="AV1" s="2" t="inlineStr">
+        <is>
+          <t>SAPVCapitalCost50W</t>
+        </is>
+      </c>
+      <c r="AW1" s="2" t="inlineStr">
+        <is>
+          <t>SAPVCapitalCost20W</t>
+        </is>
+      </c>
+      <c r="AX1" s="2" t="inlineStr">
+        <is>
           <t>MGDieselOMofTDLines</t>
         </is>
       </c>
-      <c r="AU1" s="2" t="inlineStr">
+      <c r="AY1" s="2" t="inlineStr">
         <is>
           <t>MGDieselDistributionLosses</t>
         </is>
       </c>
-      <c r="AV1" s="2" t="inlineStr">
+      <c r="AZ1" s="2" t="inlineStr">
         <is>
           <t>MGDieselConnectionCostPerHH</t>
         </is>
       </c>
-      <c r="AW1" s="2" t="inlineStr">
+      <c r="BA1" s="2" t="inlineStr">
         <is>
           <t>MGDieselBaseToPeakLoadRatio</t>
         </is>
       </c>
-      <c r="AX1" s="2" t="inlineStr">
+      <c r="BB1" s="2" t="inlineStr">
         <is>
           <t>MGDieselCapitalCost</t>
         </is>
       </c>
-      <c r="AY1" s="2" t="inlineStr">
+      <c r="BC1" s="2" t="inlineStr">
         <is>
           <t>MGDieselOMCosts</t>
         </is>
       </c>
-      <c r="AZ1" s="2" t="inlineStr">
+      <c r="BD1" s="2" t="inlineStr">
         <is>
           <t>MGDieselTechnicalLife</t>
         </is>
       </c>
-      <c r="BA1" s="2" t="inlineStr">
+      <c r="BE1" s="2" t="inlineStr">
         <is>
           <t>MGDieselCapacityFactor</t>
         </is>
       </c>
-      <c r="BB1" s="2" t="inlineStr">
+      <c r="BF1" s="2" t="inlineStr">
         <is>
           <t>SADieselBaseToPeakLoadRatio</t>
         </is>
       </c>
-      <c r="BC1" s="2" t="inlineStr">
+      <c r="BG1" s="2" t="inlineStr">
         <is>
           <t>SADieselTechnicalLife</t>
         </is>
       </c>
-      <c r="BD1" s="2" t="inlineStr">
+      <c r="BH1" s="2" t="inlineStr">
         <is>
           <t>SADieselOMCosts</t>
         </is>
       </c>
-      <c r="BE1" s="2" t="inlineStr">
+      <c r="BI1" s="2" t="inlineStr">
         <is>
           <t>SADieselCapitalCost</t>
         </is>
       </c>
-      <c r="BF1" s="2" t="inlineStr">
+      <c r="BJ1" s="2" t="inlineStr">
         <is>
           <t>SADieselCapacityFactor</t>
         </is>
       </c>
-      <c r="BG1" s="2" t="inlineStr">
+      <c r="BK1" s="2" t="inlineStr">
         <is>
           <t>SADieselEfficiency</t>
         </is>
       </c>
-      <c r="BH1" s="2" t="inlineStr">
+      <c r="BL1" s="2" t="inlineStr">
         <is>
           <t>SADieselTruckConsumption</t>
         </is>
       </c>
-      <c r="BI1" s="2" t="inlineStr">
+      <c r="BM1" s="2" t="inlineStr">
         <is>
           <t>SADieselTruckVolume</t>
         </is>
       </c>
-      <c r="BJ1" s="2" t="inlineStr">
+      <c r="BN1" s="2" t="inlineStr">
         <is>
           <t>MGDieselEfficiency</t>
         </is>
       </c>
-      <c r="BK1" s="2" t="inlineStr">
+      <c r="BO1" s="2" t="inlineStr">
         <is>
           <t>MGDieselTruckConsumption</t>
         </is>
       </c>
-      <c r="BL1" s="2" t="inlineStr">
+      <c r="BP1" s="2" t="inlineStr">
         <is>
           <t>MGDieselTruckVolume</t>
         </is>
@@ -2093,7 +2108,7 @@
         <v>9999</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1563525819208897</v>
+        <v>0.1442555788468982</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -2141,7 +2156,7 @@
         <v>0.85</v>
       </c>
       <c r="X2" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="Y2" t="n">
         <v>0.35</v>
@@ -2165,7 +2180,7 @@
         <v>0.85</v>
       </c>
       <c r="AF2" t="n">
-        <v>1219.4</v>
+        <v>2800</v>
       </c>
       <c r="AG2" t="n">
         <v>0.04</v>
@@ -2204,63 +2219,75 @@
         <v>0.013</v>
       </c>
       <c r="AS2" t="n">
-        <v>1033.4</v>
+        <v>6950</v>
       </c>
       <c r="AT2" t="n">
+        <v>4470</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>6380</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>8780</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>9620</v>
+      </c>
+      <c r="AX2" t="n">
         <v>1e-06</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="AY2" t="n">
         <v>0.05</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="AZ2" t="n">
         <v>100</v>
       </c>
-      <c r="AW2" t="n">
+      <c r="BA2" t="n">
         <v>0.85</v>
       </c>
-      <c r="AX2" t="n">
-        <v>750</v>
-      </c>
-      <c r="AY2" t="n">
+      <c r="BB2" t="n">
+        <v>261</v>
+      </c>
+      <c r="BC2" t="n">
         <v>0.03</v>
       </c>
-      <c r="AZ2" t="n">
+      <c r="BD2" t="n">
         <v>25</v>
       </c>
-      <c r="BA2" t="n">
+      <c r="BE2" t="n">
         <v>0.7</v>
-      </c>
-      <c r="BB2" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>25</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>750</v>
       </c>
       <c r="BF2" t="n">
         <v>0.9</v>
       </c>
       <c r="BG2" t="n">
+        <v>25</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>261</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BK2" t="n">
         <v>0.16</v>
       </c>
-      <c r="BH2" t="n">
+      <c r="BL2" t="n">
         <v>14</v>
       </c>
-      <c r="BI2" t="n">
+      <c r="BM2" t="n">
         <v>300</v>
       </c>
-      <c r="BJ2" t="n">
+      <c r="BN2" t="n">
         <v>0.35</v>
       </c>
-      <c r="BK2" t="n">
+      <c r="BO2" t="n">
         <v>33.7</v>
       </c>
-      <c r="BL2" t="n">
+      <c r="BP2" t="n">
         <v>15000</v>
       </c>
     </row>
@@ -2287,7 +2314,7 @@
         <v>9999</v>
       </c>
       <c r="H3" t="n">
-        <v>0.08477266592724483</v>
+        <v>0.1028339888476067</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -2335,7 +2362,7 @@
         <v>0.85</v>
       </c>
       <c r="X3" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="Y3" t="n">
         <v>0.35</v>
@@ -2359,7 +2386,7 @@
         <v>0.85</v>
       </c>
       <c r="AF3" t="n">
-        <v>963.8</v>
+        <v>2213.08840413318</v>
       </c>
       <c r="AG3" t="n">
         <v>0.04</v>
@@ -2398,63 +2425,75 @@
         <v>0.013</v>
       </c>
       <c r="AS3" t="n">
-        <v>794.1</v>
+        <v>5340.618347203406</v>
       </c>
       <c r="AT3" t="n">
+        <v>3434.901296690536</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>4902.61079930327</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>6746.853106251209</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>7392.337913682988</v>
+      </c>
+      <c r="AX3" t="n">
         <v>1e-06</v>
       </c>
-      <c r="AU3" t="n">
+      <c r="AY3" t="n">
         <v>0.05</v>
       </c>
-      <c r="AV3" t="n">
+      <c r="AZ3" t="n">
         <v>100</v>
       </c>
-      <c r="AW3" t="n">
+      <c r="BA3" t="n">
         <v>0.85</v>
       </c>
-      <c r="AX3" t="n">
-        <v>750</v>
-      </c>
-      <c r="AY3" t="n">
+      <c r="BB3" t="n">
+        <v>261</v>
+      </c>
+      <c r="BC3" t="n">
         <v>0.03</v>
       </c>
-      <c r="AZ3" t="n">
+      <c r="BD3" t="n">
         <v>25</v>
       </c>
-      <c r="BA3" t="n">
+      <c r="BE3" t="n">
         <v>0.7</v>
-      </c>
-      <c r="BB3" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="BC3" t="n">
-        <v>25</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>750</v>
       </c>
       <c r="BF3" t="n">
         <v>0.9</v>
       </c>
       <c r="BG3" t="n">
+        <v>25</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>261</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BK3" t="n">
         <v>0.16</v>
       </c>
-      <c r="BH3" t="n">
+      <c r="BL3" t="n">
         <v>14</v>
       </c>
-      <c r="BI3" t="n">
+      <c r="BM3" t="n">
         <v>300</v>
       </c>
-      <c r="BJ3" t="n">
+      <c r="BN3" t="n">
         <v>0.35</v>
       </c>
-      <c r="BK3" t="n">
+      <c r="BO3" t="n">
         <v>33.7</v>
       </c>
-      <c r="BL3" t="n">
+      <c r="BP3" t="n">
         <v>15000</v>
       </c>
     </row>
@@ -2481,7 +2520,7 @@
         <v>9999</v>
       </c>
       <c r="H4" t="n">
-        <v>0.06908486338395285</v>
+        <v>0.07066136907172905</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -2529,7 +2568,7 @@
         <v>0.85</v>
       </c>
       <c r="X4" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="Y4" t="n">
         <v>0.35</v>
@@ -2553,7 +2592,7 @@
         <v>0.85</v>
       </c>
       <c r="AF4" t="n">
-        <v>933</v>
+        <v>2142.365097588978</v>
       </c>
       <c r="AG4" t="n">
         <v>0.04</v>
@@ -2592,63 +2631,75 @@
         <v>0.013</v>
       </c>
       <c r="AS4" t="n">
-        <v>723</v>
+        <v>4862.444358428489</v>
       </c>
       <c r="AT4" t="n">
+        <v>3127.356299593574</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>4463.653957809173</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>6142.771434101026</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>6730.462550803174</v>
+      </c>
+      <c r="AX4" t="n">
         <v>1e-06</v>
       </c>
-      <c r="AU4" t="n">
+      <c r="AY4" t="n">
         <v>0.05</v>
       </c>
-      <c r="AV4" t="n">
+      <c r="AZ4" t="n">
         <v>100</v>
       </c>
-      <c r="AW4" t="n">
+      <c r="BA4" t="n">
         <v>0.85</v>
       </c>
-      <c r="AX4" t="n">
-        <v>750</v>
-      </c>
-      <c r="AY4" t="n">
+      <c r="BB4" t="n">
+        <v>261</v>
+      </c>
+      <c r="BC4" t="n">
         <v>0.03</v>
       </c>
-      <c r="AZ4" t="n">
+      <c r="BD4" t="n">
         <v>25</v>
       </c>
-      <c r="BA4" t="n">
+      <c r="BE4" t="n">
         <v>0.7</v>
-      </c>
-      <c r="BB4" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="BC4" t="n">
-        <v>25</v>
-      </c>
-      <c r="BD4" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>750</v>
       </c>
       <c r="BF4" t="n">
         <v>0.9</v>
       </c>
       <c r="BG4" t="n">
+        <v>25</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>261</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BK4" t="n">
         <v>0.16</v>
       </c>
-      <c r="BH4" t="n">
+      <c r="BL4" t="n">
         <v>14</v>
       </c>
-      <c r="BI4" t="n">
+      <c r="BM4" t="n">
         <v>300</v>
       </c>
-      <c r="BJ4" t="n">
+      <c r="BN4" t="n">
         <v>0.35</v>
       </c>
-      <c r="BK4" t="n">
+      <c r="BO4" t="n">
         <v>33.7</v>
       </c>
-      <c r="BL4" t="n">
+      <c r="BP4" t="n">
         <v>15000</v>
       </c>
     </row>
@@ -2675,7 +2726,7 @@
         <v>9999</v>
       </c>
       <c r="H5" t="n">
-        <v>0.04666558794496197</v>
+        <v>0.03077546979549152</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -2723,7 +2774,7 @@
         <v>0.85</v>
       </c>
       <c r="X5" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="Y5" t="n">
         <v>0.35</v>
@@ -2747,7 +2798,7 @@
         <v>0.85</v>
       </c>
       <c r="AF5" t="n">
-        <v>933</v>
+        <v>2142.365097588978</v>
       </c>
       <c r="AG5" t="n">
         <v>0.04</v>
@@ -2786,63 +2837,75 @@
         <v>0.013</v>
       </c>
       <c r="AS5" t="n">
-        <v>723</v>
+        <v>4862.444358428489</v>
       </c>
       <c r="AT5" t="n">
+        <v>3127.356299593574</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>4463.653957809173</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>6142.771434101026</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>6730.462550803174</v>
+      </c>
+      <c r="AX5" t="n">
         <v>1e-06</v>
       </c>
-      <c r="AU5" t="n">
+      <c r="AY5" t="n">
         <v>0.05</v>
       </c>
-      <c r="AV5" t="n">
+      <c r="AZ5" t="n">
         <v>100</v>
       </c>
-      <c r="AW5" t="n">
+      <c r="BA5" t="n">
         <v>0.85</v>
       </c>
-      <c r="AX5" t="n">
-        <v>750</v>
-      </c>
-      <c r="AY5" t="n">
+      <c r="BB5" t="n">
+        <v>261</v>
+      </c>
+      <c r="BC5" t="n">
         <v>0.03</v>
       </c>
-      <c r="AZ5" t="n">
+      <c r="BD5" t="n">
         <v>25</v>
       </c>
-      <c r="BA5" t="n">
+      <c r="BE5" t="n">
         <v>0.7</v>
-      </c>
-      <c r="BB5" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="BC5" t="n">
-        <v>25</v>
-      </c>
-      <c r="BD5" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="BE5" t="n">
-        <v>750</v>
       </c>
       <c r="BF5" t="n">
         <v>0.9</v>
       </c>
       <c r="BG5" t="n">
+        <v>25</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>261</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BK5" t="n">
         <v>0.16</v>
       </c>
-      <c r="BH5" t="n">
+      <c r="BL5" t="n">
         <v>14</v>
       </c>
-      <c r="BI5" t="n">
+      <c r="BM5" t="n">
         <v>300</v>
       </c>
-      <c r="BJ5" t="n">
+      <c r="BN5" t="n">
         <v>0.35</v>
       </c>
-      <c r="BK5" t="n">
+      <c r="BO5" t="n">
         <v>33.7</v>
       </c>
-      <c r="BL5" t="n">
+      <c r="BP5" t="n">
         <v>15000</v>
       </c>
     </row>
@@ -2869,7 +2932,7 @@
         <v>9999</v>
       </c>
       <c r="H6" t="n">
-        <v>0.02430517192505205</v>
+        <v>0.0128761301770414</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -2917,7 +2980,7 @@
         <v>0.85</v>
       </c>
       <c r="X6" t="n">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="Y6" t="n">
         <v>0.35</v>
@@ -2941,7 +3004,7 @@
         <v>0.85</v>
       </c>
       <c r="AF6" t="n">
-        <v>933</v>
+        <v>2142.365097588978</v>
       </c>
       <c r="AG6" t="n">
         <v>0.04</v>
@@ -2980,63 +3043,75 @@
         <v>0.013</v>
       </c>
       <c r="AS6" t="n">
-        <v>723</v>
+        <v>4862.444358428489</v>
       </c>
       <c r="AT6" t="n">
+        <v>3127.356299593574</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>4463.653957809173</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>6142.771434101026</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>6730.462550803174</v>
+      </c>
+      <c r="AX6" t="n">
         <v>1e-06</v>
       </c>
-      <c r="AU6" t="n">
+      <c r="AY6" t="n">
         <v>0.05</v>
       </c>
-      <c r="AV6" t="n">
+      <c r="AZ6" t="n">
         <v>100</v>
       </c>
-      <c r="AW6" t="n">
+      <c r="BA6" t="n">
         <v>0.85</v>
       </c>
-      <c r="AX6" t="n">
-        <v>750</v>
-      </c>
-      <c r="AY6" t="n">
+      <c r="BB6" t="n">
+        <v>261</v>
+      </c>
+      <c r="BC6" t="n">
         <v>0.03</v>
       </c>
-      <c r="AZ6" t="n">
+      <c r="BD6" t="n">
         <v>25</v>
       </c>
-      <c r="BA6" t="n">
+      <c r="BE6" t="n">
         <v>0.7</v>
-      </c>
-      <c r="BB6" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="BC6" t="n">
-        <v>25</v>
-      </c>
-      <c r="BD6" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="BE6" t="n">
-        <v>750</v>
       </c>
       <c r="BF6" t="n">
         <v>0.9</v>
       </c>
       <c r="BG6" t="n">
+        <v>25</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>261</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BK6" t="n">
         <v>0.16</v>
       </c>
-      <c r="BH6" t="n">
+      <c r="BL6" t="n">
         <v>14</v>
       </c>
-      <c r="BI6" t="n">
+      <c r="BM6" t="n">
         <v>300</v>
       </c>
-      <c r="BJ6" t="n">
+      <c r="BN6" t="n">
         <v>0.35</v>
       </c>
-      <c r="BK6" t="n">
+      <c r="BO6" t="n">
         <v>33.7</v>
       </c>
-      <c r="BL6" t="n">
+      <c r="BP6" t="n">
         <v>15000</v>
       </c>
     </row>
@@ -3281,7 +3356,7 @@
         <v>27382000</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3711499869823456</v>
+        <v>0.371149986982346</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -3316,13 +3391,13 @@
         <v>9999</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9499095925348843</v>
+        <v>0.9499996205318469</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9788991087445169</v>
+        <v>0.9204893317023679</v>
       </c>
       <c r="V3" t="n">
-        <v>0.9007920231165003</v>
+        <v>0.9999999236071855</v>
       </c>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
@@ -3352,7 +3427,7 @@
         <v>34954000</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4372100234031677</v>
+        <v>0.437210023403168</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -3423,7 +3498,7 @@
         <v>43207000</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5017101168632507</v>
+        <v>0.501710116863251</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
@@ -3494,7 +3569,7 @@
         <v>52504270</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5701609253883362</v>
+        <v>0.570160925388336</v>
       </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>

</xml_diff>